<commit_message>
- Adding new things to check with legal - Fixed issue rendering html in the table (icons) - Changed line height to normal not zero - Cleaned up some examples - Added an example of a menu button on a toolbar
</commit_message>
<xml_diff>
--- a/SoHo XI.xlsx
+++ b/SoHo XI.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-42680" yWindow="-11120" windowWidth="32860" windowHeight="18440" tabRatio="858" activeTab="5"/>
+    <workbookView xWindow="-9060" yWindow="-24640" windowWidth="25600" windowHeight="16060" tabRatio="858" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Open Source Policy" sheetId="4" r:id="rId1"/>
@@ -1750,7 +1750,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="151">
   <si>
     <t>MODIFICATION HISTORY</t>
   </si>
@@ -2437,9 +2437,6 @@
     <t>Grunt Js</t>
   </si>
   <si>
-    <t>.0.4.1</t>
-  </si>
-  <si>
     <t>Used to build Infor Source Code</t>
   </si>
   <si>
@@ -2462,6 +2459,18 @@
   </si>
   <si>
     <t>Used to build and Test and Host Infor Source Code</t>
+  </si>
+  <si>
+    <t>Hogan</t>
+  </si>
+  <si>
+    <t>Rivets</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>0.4.1</t>
   </si>
 </sst>
 </file>
@@ -8663,7 +8672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0"/>
@@ -8924,7 +8933,7 @@
         <v>133</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F8" s="86" t="s">
         <v>107</v>
@@ -8957,7 +8966,7 @@
         <v>138</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C9" s="118">
         <v>41576</v>
@@ -8966,7 +8975,7 @@
         <v>137</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F9" s="86" t="s">
         <v>109</v>
@@ -8978,10 +8987,10 @@
         <v>109</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>109</v>
@@ -8996,19 +9005,19 @@
     </row>
     <row r="10" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
       <c r="A10" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" t="s">
         <v>143</v>
-      </c>
-      <c r="B10" t="s">
-        <v>144</v>
       </c>
       <c r="C10" s="118">
         <v>41576</v>
       </c>
       <c r="D10" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>146</v>
       </c>
       <c r="F10" s="86" t="s">
         <v>109</v>
@@ -9020,10 +9029,10 @@
         <v>109</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>109</v>
@@ -9037,6 +9046,9 @@
       <c r="N10" s="15"/>
     </row>
     <row r="11" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+      <c r="A11" s="14" t="s">
+        <v>147</v>
+      </c>
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
       <c r="D11" s="46"/>
@@ -9045,6 +9057,9 @@
       <c r="N11" s="15"/>
     </row>
     <row r="12" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+      <c r="A12" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="B12" s="46"/>
       <c r="C12" s="46"/>
       <c r="D12" s="46"/>
@@ -9053,6 +9068,9 @@
       <c r="N12" s="15"/>
     </row>
     <row r="13" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+      <c r="A13" s="14" t="s">
+        <v>149</v>
+      </c>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
       <c r="D13" s="46"/>

</xml_diff>

<commit_message>
- Updated Change Log
</commit_message>
<xml_diff>
--- a/SoHo XI.xlsx
+++ b/SoHo XI.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmcconechy/Dev/controls/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-9060" yWindow="-24640" windowWidth="25600" windowHeight="16060" tabRatio="858" activeTab="5"/>
+    <workbookView xWindow="-38960" yWindow="-14340" windowWidth="34860" windowHeight="21200" tabRatio="858" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Open Source Policy" sheetId="4" r:id="rId1"/>
@@ -12,11 +17,15 @@
     <sheet name="History and Approvals" sheetId="2" r:id="rId3"/>
     <sheet name="Open Source Survey" sheetId="1" r:id="rId4"/>
     <sheet name="Infor Html5 Controls v3.0" sheetId="6" r:id="rId5"/>
-    <sheet name="Infor Html5 Controls v3.2" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId7"/>
+    <sheet name="Infor Html5 Controls v3.2" sheetId="8" r:id="rId6"/>
+    <sheet name="Infor Html5 Controls v4.2.1" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1749,8 +1758,583 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Andrew Hall</author>
+  </authors>
+  <commentList>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A. OSS Component</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Please provide the names of the OSS Components used or distributed in connection with our Product, including any development tools (e.g., debuggers, compilers, SDKs), libraries, applications, and other OSS Components.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>B. OSS Version</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Please provide the version numbers for the OSS Component.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>C. Date</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Please provide the date that the OSS Component was last downloaded and placed into the company's software repository.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">D. Provider/Source
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Please provide the hypertext link (URL) to the website, ftp site, or other source of the OSS Components.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E. License/Link</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Please identify the applicable OSS License (e.g., Apache 2.0, LGPL 2.1) and  provide link (URL) directly to the OSS license terms covering the Component.  
+Do NOT provide a link to the to source of OSS, which is to be provided in Column D; instead, link directly to the OSS license terms. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">F. Sub-Components  </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If the OSS Component is a sub-component of another OSS Component or includes other OSS Components, please identify those OSS Components and the relationship between the OSS Components.  (e.g., OSS Component A incorporates/depends on OSS Component B)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>G. Distribution</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+NOTE: THIS IS A 2-PART QUESTION. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Part 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.  Please indicate, with a "</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YES</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>" or "</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">", whether this OSS Component will be distributed to Infor customers or others outside the company.  Please note that providing access to the software in a hosted environment, but not providing a copy of the software, does not constitute distribution.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Part 2. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> If the answer to Part 1 is "</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YES</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">", please describe how the OSS Components will be distributed by Info outside the company, by picking the appropriate a letter below or by providing a description of the distribution.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(A)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Infor will be providing the OSS as a bundled, embedded or linked module to the Infor software.   
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(B)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Infor will be providing the OSS as a standalone, separate program. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(C)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> The customer will be directed to a separate site for a separate download of the OSS. 
+For example, if Infor provides the OSS Component embedded within Infor products, the entry for such component is "</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YES (A)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">".
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">H. Redistribution </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Please indicate whether the OSS Component will be redistributed by our customer or others outside the Company.  </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+(Typically, the answer here should be NO)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>I. Interaction with Company Code</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Please indicate how the OSS Component will interact with the Infor Product(s).  
+Examples of interaction descriptions include: 
+(i) OSS is a standalone program, 
+(ii) OSS statically linked to, 
+(iii) OSS dynamically linked to,
+(iv) OSS directly combined with Infor source code, 
+(v) OSS passes data to Infor software through files.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>J. Purpose</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Describe the purpose for using the OSS Component.
+Examples of purpose descriptions include:
+(i) Web server
+(ii) PDF creation/ manipulation
+(iii) Data encryption
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>L. Modifications.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Please indicate whether any modifications have been or will be made to the OSS.  If so, please describe the nature of those modifications.  
+Examples of modification descriptions include:
+(i) bug fixes,
+(ii) functional enhancements,
+(iii) ported to another platform.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note: Written Approval Required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Infor's current OSS Policy does NOT permit contributions without specific written approval. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Note: Do NOT Remove Notices from OSS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Copyright notices, disclaimers, and similar notices should NOT be removed from the OSS source code or other OSS materials.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">In addition to the requirements set forth below, most OSS license terms require inclusion of the appropriate copyright notices, notices of attribution to the author, and a copy of the OSS license, including all required disclaimers, as set forth in the OSS license agreement. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="152">
   <si>
     <t>MODIFICATION HISTORY</t>
   </si>
@@ -2461,16 +3045,19 @@
     <t>Used to build and Test and Host Infor Source Code</t>
   </si>
   <si>
-    <t>Hogan</t>
-  </si>
-  <si>
-    <t>Rivets</t>
-  </si>
-  <si>
-    <t>Angular</t>
-  </si>
-  <si>
     <t>0.4.1</t>
+  </si>
+  <si>
+    <t>3.1.0</t>
+  </si>
+  <si>
+    <t>Cheryl Brinkman</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Changed Jquery Version, Removed Dev only Dependencies and added new Tab for 4.2.1</t>
   </si>
 </sst>
 </file>
@@ -2903,7 +3490,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -3272,6 +3859,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -5968,14 +6558,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -6285,9 +6875,9 @@
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="2:17">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B1" s="57"/>
       <c r="C1" s="58"/>
       <c r="D1" s="58"/>
@@ -6307,7 +6897,7 @@
       <c r="P1" s="58"/>
       <c r="Q1" s="59"/>
     </row>
-    <row r="2" spans="2:17">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B2" s="60"/>
       <c r="C2" s="56"/>
       <c r="D2" s="56"/>
@@ -6327,7 +6917,7 @@
       <c r="P2" s="56"/>
       <c r="Q2" s="62"/>
     </row>
-    <row r="3" spans="2:17">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B3" s="63"/>
       <c r="C3" s="64"/>
       <c r="D3" s="64"/>
@@ -6351,11 +6941,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6367,7 +6952,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="143.6640625" style="24" customWidth="1"/>
@@ -6563,7 +7148,7 @@
     <col min="16131" max="16384" width="8.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="18" customFormat="1" ht="17">
+    <row r="1" spans="2:8" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="B1" s="19" t="s">
         <v>18</v>
       </c>
@@ -6574,128 +7159,128 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="2:8" s="21" customFormat="1" ht="24" customHeight="1">
+    <row r="2" spans="2:8" s="21" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="6" customHeight="1"/>
-    <row r="4" spans="2:8" ht="16" thickBot="1">
+    <row r="3" spans="2:8" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="4" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="26" customFormat="1" ht="9">
+    <row r="5" spans="2:8" s="26" customFormat="1" ht="9" x14ac:dyDescent="0.15">
       <c r="B5" s="27"/>
     </row>
-    <row r="6" spans="2:8" ht="33.75" customHeight="1">
+    <row r="6" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="26" customFormat="1" ht="9">
+    <row r="7" spans="2:8" s="26" customFormat="1" ht="9" x14ac:dyDescent="0.15">
       <c r="B7" s="27"/>
     </row>
-    <row r="8" spans="2:8" ht="26.25" customHeight="1">
+    <row r="8" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="26" customFormat="1" ht="7.5" customHeight="1">
+    <row r="9" spans="2:8" s="26" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="27"/>
     </row>
-    <row r="10" spans="2:8" ht="33.75" customHeight="1">
+    <row r="10" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="26" customFormat="1" ht="7.5" customHeight="1">
+    <row r="11" spans="2:8" s="26" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="27"/>
     </row>
-    <row r="12" spans="2:8" ht="41.25" customHeight="1">
+    <row r="12" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B13" s="30"/>
     </row>
-    <row r="14" spans="2:8" ht="24">
+    <row r="14" spans="2:8" ht="26" x14ac:dyDescent="0.15">
       <c r="B14" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B15" s="30"/>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B16" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="29" customFormat="1" ht="16" thickBot="1">
+    <row r="18" spans="2:2" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:2" s="26" customFormat="1" ht="5.25" customHeight="1">
+    <row r="19" spans="2:2" s="26" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="27"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:2" s="26" customFormat="1" ht="5.25" customHeight="1">
+    <row r="21" spans="2:2" s="26" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="27"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B23" s="28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B25" s="31"/>
     </row>
-    <row r="26" spans="2:2" s="29" customFormat="1" ht="16" thickBot="1">
+    <row r="26" spans="2:2" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B26" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="34.5" customHeight="1">
+    <row r="27" spans="2:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="34.5" customHeight="1">
+    <row r="28" spans="2:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="30"/>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B29" s="30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B31" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B35" s="68" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B36" s="67" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B37" s="69" t="s">
         <v>48</v>
       </c>
@@ -6708,11 +7293,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6720,11 +7300,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="62.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -6733,7 +7313,7 @@
     <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="51"/>
       <c r="B1" s="51"/>
       <c r="C1" s="52" t="s">
@@ -6743,7 +7323,7 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="53" t="s">
@@ -6753,7 +7333,7 @@
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:6" ht="21">
+    <row r="3" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A3" s="119" t="s">
         <v>0</v>
       </c>
@@ -6763,14 +7343,14 @@
       <c r="E3" s="120"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="1:6" ht="13" thickBot="1">
+    <row r="4" spans="1:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="16" thickTop="1" thickBot="1">
+    <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -6790,7 +7370,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14" thickTop="1">
+    <row r="6" spans="1:6" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A6" s="89" t="s">
         <v>113</v>
       </c>
@@ -6810,7 +7390,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>114</v>
       </c>
@@ -6828,7 +7408,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>
       <c r="B8" s="5"/>
       <c r="C8" s="91" t="s">
@@ -6837,20 +7417,26 @@
       <c r="D8" s="92" t="s">
         <v>136</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="121" t="s">
         <v>135</v>
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="11"/>
+      <c r="C9" s="91" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="121" t="s">
+        <v>151</v>
+      </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="5"/>
       <c r="C10" s="11"/>
@@ -6858,7 +7444,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="7"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
@@ -6866,7 +7452,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="7"/>
       <c r="B12" s="5"/>
       <c r="C12" s="11"/>
@@ -6874,7 +7460,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="7"/>
       <c r="B13" s="5"/>
       <c r="C13" s="8"/>
@@ -6882,7 +7468,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="7"/>
       <c r="B14" s="5"/>
       <c r="C14" s="8"/>
@@ -6898,11 +7484,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="75" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6918,7 +7499,7 @@
       <selection pane="bottomLeft" activeCell="B17" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="35.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" style="48" customWidth="1"/>
@@ -6937,7 +7518,7 @@
     <col min="15" max="16384" width="9.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="80" t="s">
         <v>55</v>
       </c>
@@ -6955,7 +7536,7 @@
       <c r="M1" s="54"/>
       <c r="N1" s="55"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="82" t="s">
         <v>56</v>
       </c>
@@ -6973,7 +7554,7 @@
       <c r="M2" s="54"/>
       <c r="N2" s="55"/>
     </row>
-    <row r="3" spans="1:14" s="38" customFormat="1" ht="19">
+    <row r="3" spans="1:14" s="38" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
         <v>14</v>
       </c>
@@ -6986,7 +7567,7 @@
       <c r="F3" s="43"/>
       <c r="N3" s="39"/>
     </row>
-    <row r="4" spans="1:14" s="42" customFormat="1" ht="36.75" customHeight="1">
+    <row r="4" spans="1:14" s="42" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
         <v>43</v>
       </c>
@@ -7030,7 +7611,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="43.5" customHeight="1">
+    <row r="5" spans="1:14" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="34" t="s">
         <v>36</v>
       </c>
@@ -7074,7 +7655,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="14" customFormat="1" ht="38.25" customHeight="1">
+    <row r="6" spans="1:14" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -7090,7 +7671,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="15"/>
     </row>
-    <row r="7" spans="1:14" s="14" customFormat="1">
+    <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -7106,7 +7687,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="15"/>
     </row>
-    <row r="8" spans="1:14" s="14" customFormat="1">
+    <row r="8" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -7122,7 +7703,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="15"/>
     </row>
-    <row r="9" spans="1:14" s="14" customFormat="1">
+    <row r="9" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -7138,7 +7719,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="15"/>
     </row>
-    <row r="10" spans="1:14" s="14" customFormat="1">
+    <row r="10" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -7154,7 +7735,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="15"/>
     </row>
-    <row r="11" spans="1:14" s="14" customFormat="1">
+    <row r="11" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -7170,7 +7751,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="15"/>
     </row>
-    <row r="12" spans="1:14" s="14" customFormat="1">
+    <row r="12" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -7186,7 +7767,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="15"/>
     </row>
-    <row r="13" spans="1:14" s="14" customFormat="1">
+    <row r="13" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -7202,7 +7783,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="15"/>
     </row>
-    <row r="14" spans="1:14" s="14" customFormat="1">
+    <row r="14" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -7218,7 +7799,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="15"/>
     </row>
-    <row r="15" spans="1:14" s="14" customFormat="1">
+    <row r="15" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
       <c r="D15" s="46"/>
@@ -7233,7 +7814,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="15"/>
     </row>
-    <row r="16" spans="1:14" s="14" customFormat="1">
+    <row r="16" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
       <c r="D16" s="46"/>
@@ -7248,7 +7829,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="2:14" s="14" customFormat="1">
+    <row r="17" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="46"/>
       <c r="C17" s="46"/>
       <c r="D17" s="46"/>
@@ -7263,7 +7844,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="2:14" s="14" customFormat="1">
+    <row r="18" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
       <c r="D18" s="46"/>
@@ -7278,7 +7859,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="15"/>
     </row>
-    <row r="19" spans="2:14" s="14" customFormat="1">
+    <row r="19" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
       <c r="D19" s="46"/>
@@ -7293,7 +7874,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="15"/>
     </row>
-    <row r="20" spans="2:14" s="14" customFormat="1">
+    <row r="20" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B20" s="46"/>
       <c r="C20" s="46"/>
       <c r="D20" s="46"/>
@@ -7308,7 +7889,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="15"/>
     </row>
-    <row r="21" spans="2:14" s="14" customFormat="1">
+    <row r="21" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B21" s="46"/>
       <c r="C21" s="46"/>
       <c r="D21" s="46"/>
@@ -7323,7 +7904,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="15"/>
     </row>
-    <row r="22" spans="2:14" s="14" customFormat="1">
+    <row r="22" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="46"/>
       <c r="C22" s="46"/>
       <c r="D22" s="46"/>
@@ -7338,119 +7919,119 @@
       <c r="M22" s="1"/>
       <c r="N22" s="15"/>
     </row>
-    <row r="23" spans="2:14" s="14" customFormat="1">
+    <row r="23" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B23" s="46"/>
       <c r="C23" s="46"/>
       <c r="D23" s="46"/>
       <c r="F23" s="47"/>
       <c r="N23" s="15"/>
     </row>
-    <row r="24" spans="2:14" s="14" customFormat="1">
+    <row r="24" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B24" s="46"/>
       <c r="C24" s="46"/>
       <c r="D24" s="46"/>
       <c r="F24" s="47"/>
       <c r="N24" s="15"/>
     </row>
-    <row r="25" spans="2:14" s="14" customFormat="1">
+    <row r="25" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
       <c r="F25" s="47"/>
       <c r="N25" s="15"/>
     </row>
-    <row r="26" spans="2:14" s="14" customFormat="1">
+    <row r="26" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B26" s="46"/>
       <c r="C26" s="46"/>
       <c r="D26" s="46"/>
       <c r="F26" s="47"/>
       <c r="N26" s="15"/>
     </row>
-    <row r="27" spans="2:14" s="14" customFormat="1">
+    <row r="27" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B27" s="46"/>
       <c r="C27" s="46"/>
       <c r="D27" s="46"/>
       <c r="F27" s="47"/>
       <c r="N27" s="15"/>
     </row>
-    <row r="28" spans="2:14" s="14" customFormat="1">
+    <row r="28" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
       <c r="D28" s="46"/>
       <c r="F28" s="47"/>
       <c r="N28" s="15"/>
     </row>
-    <row r="29" spans="2:14" s="14" customFormat="1">
+    <row r="29" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B29" s="46"/>
       <c r="C29" s="46"/>
       <c r="D29" s="46"/>
       <c r="F29" s="47"/>
       <c r="N29" s="15"/>
     </row>
-    <row r="30" spans="2:14" s="14" customFormat="1">
+    <row r="30" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B30" s="46"/>
       <c r="C30" s="46"/>
       <c r="D30" s="46"/>
       <c r="F30" s="47"/>
       <c r="N30" s="15"/>
     </row>
-    <row r="31" spans="2:14" s="14" customFormat="1">
+    <row r="31" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
       <c r="D31" s="46"/>
       <c r="F31" s="47"/>
       <c r="N31" s="15"/>
     </row>
-    <row r="32" spans="2:14" s="14" customFormat="1">
+    <row r="32" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B32" s="46"/>
       <c r="C32" s="46"/>
       <c r="D32" s="46"/>
       <c r="F32" s="47"/>
       <c r="N32" s="15"/>
     </row>
-    <row r="33" spans="1:14" s="14" customFormat="1">
+    <row r="33" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B33" s="46"/>
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
       <c r="F33" s="47"/>
       <c r="N33" s="15"/>
     </row>
-    <row r="34" spans="1:14" s="14" customFormat="1">
+    <row r="34" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
       <c r="D34" s="46"/>
       <c r="F34" s="47"/>
       <c r="N34" s="15"/>
     </row>
-    <row r="35" spans="1:14" s="14" customFormat="1">
+    <row r="35" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B35" s="46"/>
       <c r="C35" s="46"/>
       <c r="D35" s="46"/>
       <c r="F35" s="47"/>
       <c r="N35" s="15"/>
     </row>
-    <row r="36" spans="1:14" s="14" customFormat="1">
+    <row r="36" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B36" s="46"/>
       <c r="C36" s="46"/>
       <c r="D36" s="46"/>
       <c r="F36" s="47"/>
       <c r="N36" s="15"/>
     </row>
-    <row r="37" spans="1:14" s="14" customFormat="1">
+    <row r="37" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B37" s="46"/>
       <c r="C37" s="46"/>
       <c r="D37" s="46"/>
       <c r="F37" s="47"/>
       <c r="N37" s="15"/>
     </row>
-    <row r="38" spans="1:14" s="14" customFormat="1">
+    <row r="38" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B38" s="46"/>
       <c r="C38" s="46"/>
       <c r="D38" s="46"/>
       <c r="F38" s="47"/>
       <c r="N38" s="15"/>
     </row>
-    <row r="39" spans="1:14" s="14" customFormat="1">
+    <row r="39" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="16"/>
       <c r="B39" s="46"/>
       <c r="C39" s="46"/>
@@ -7458,7 +8039,7 @@
       <c r="F39" s="47"/>
       <c r="N39" s="15"/>
     </row>
-    <row r="40" spans="1:14" s="14" customFormat="1">
+    <row r="40" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="16"/>
       <c r="B40" s="46"/>
       <c r="C40" s="46"/>
@@ -7466,7 +8047,7 @@
       <c r="F40" s="47"/>
       <c r="N40" s="15"/>
     </row>
-    <row r="41" spans="1:14" s="14" customFormat="1">
+    <row r="41" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="16"/>
       <c r="B41" s="46"/>
       <c r="C41" s="46"/>
@@ -7474,7 +8055,7 @@
       <c r="F41" s="47"/>
       <c r="N41" s="15"/>
     </row>
-    <row r="42" spans="1:14" s="14" customFormat="1">
+    <row r="42" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="16"/>
       <c r="B42" s="46"/>
       <c r="C42" s="46"/>
@@ -7490,11 +8071,6 @@
     <oddFooter>&amp;CCopyright © 2005 Lawson  Software Inc. all rights reserved</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7510,7 +8086,7 @@
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="35.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="48" customWidth="1"/>
@@ -7529,7 +8105,7 @@
     <col min="15" max="16384" width="9.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.5" customHeight="1">
+    <row r="1" spans="1:14" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="80" t="s">
         <v>55</v>
       </c>
@@ -7547,7 +8123,7 @@
       <c r="M1" s="54"/>
       <c r="N1" s="55"/>
     </row>
-    <row r="2" spans="1:14" ht="17.5" customHeight="1">
+    <row r="2" spans="1:14" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="82" t="s">
         <v>56</v>
       </c>
@@ -7565,7 +8141,7 @@
       <c r="M2" s="54"/>
       <c r="N2" s="55"/>
     </row>
-    <row r="3" spans="1:14" s="38" customFormat="1" ht="17" customHeight="1">
+    <row r="3" spans="1:14" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
         <v>14</v>
       </c>
@@ -7578,7 +8154,7 @@
       <c r="F3" s="43"/>
       <c r="N3" s="39"/>
     </row>
-    <row r="4" spans="1:14" s="42" customFormat="1" ht="34.25" customHeight="1">
+    <row r="4" spans="1:14" s="42" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
         <v>43</v>
       </c>
@@ -7622,7 +8198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="109" customFormat="1" ht="17.5" customHeight="1">
+    <row r="5" spans="1:14" s="109" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="106" t="s">
         <v>36</v>
       </c>
@@ -7666,7 +8242,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="6" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="93" t="s">
         <v>65</v>
       </c>
@@ -7710,7 +8286,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="7" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="93" t="s">
         <v>66</v>
       </c>
@@ -7754,7 +8330,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="8" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="93" t="s">
         <v>67</v>
       </c>
@@ -7798,7 +8374,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="9" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="93" t="s">
         <v>68</v>
       </c>
@@ -7842,7 +8418,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="10" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="93" t="s">
         <v>69</v>
       </c>
@@ -7886,7 +8462,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="11" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="93" t="s">
         <v>70</v>
       </c>
@@ -7930,7 +8506,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="12" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="102" t="s">
         <v>71</v>
       </c>
@@ -7974,7 +8550,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="13" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="102" t="s">
         <v>72</v>
       </c>
@@ -8018,7 +8594,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="14" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="102" t="s">
         <v>73</v>
       </c>
@@ -8062,7 +8638,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="15" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="102" t="s">
         <v>74</v>
       </c>
@@ -8106,7 +8682,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="16" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="102" t="s">
         <v>75</v>
       </c>
@@ -8150,7 +8726,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="17" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="102" t="s">
         <v>76</v>
       </c>
@@ -8194,7 +8770,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="18" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="102" t="s">
         <v>77</v>
       </c>
@@ -8238,7 +8814,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="19" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="102" t="s">
         <v>78</v>
       </c>
@@ -8282,7 +8858,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="20" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="102" t="s">
         <v>79</v>
       </c>
@@ -8326,7 +8902,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="21" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="102" t="s">
         <v>80</v>
       </c>
@@ -8370,7 +8946,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="22" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="102" t="s">
         <v>81</v>
       </c>
@@ -8414,7 +8990,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="23" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="102" t="s">
         <v>90</v>
       </c>
@@ -8458,7 +9034,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="24" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>132</v>
       </c>
@@ -8500,7 +9076,7 @@
       </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="25" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
@@ -8508,7 +9084,7 @@
       <c r="H25" s="1"/>
       <c r="N25" s="15"/>
     </row>
-    <row r="26" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="26" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="46"/>
       <c r="C26" s="46"/>
       <c r="D26" s="46"/>
@@ -8516,7 +9092,7 @@
       <c r="H26" s="1"/>
       <c r="N26" s="15"/>
     </row>
-    <row r="27" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="27" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="46"/>
       <c r="C27" s="46"/>
       <c r="D27" s="46"/>
@@ -8524,7 +9100,7 @@
       <c r="H27" s="1"/>
       <c r="N27" s="15"/>
     </row>
-    <row r="28" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="28" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
       <c r="D28" s="46"/>
@@ -8532,7 +9108,7 @@
       <c r="H28" s="1"/>
       <c r="N28" s="15"/>
     </row>
-    <row r="29" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="29" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="46"/>
       <c r="C29" s="46"/>
       <c r="D29" s="46"/>
@@ -8540,7 +9116,7 @@
       <c r="H29" s="87"/>
       <c r="N29" s="15"/>
     </row>
-    <row r="30" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="30" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="46"/>
       <c r="C30" s="46"/>
       <c r="D30" s="46"/>
@@ -8548,7 +9124,7 @@
       <c r="H30" s="87"/>
       <c r="N30" s="15"/>
     </row>
-    <row r="31" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="31" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
       <c r="D31" s="46"/>
@@ -8556,49 +9132,49 @@
       <c r="H31" s="87"/>
       <c r="N31" s="15"/>
     </row>
-    <row r="32" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="32" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="46"/>
       <c r="C32" s="46"/>
       <c r="D32" s="46"/>
       <c r="F32" s="47"/>
       <c r="N32" s="15"/>
     </row>
-    <row r="33" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="33" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="46"/>
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
       <c r="F33" s="47"/>
       <c r="N33" s="15"/>
     </row>
-    <row r="34" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="34" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
       <c r="D34" s="46"/>
       <c r="F34" s="47"/>
       <c r="N34" s="15"/>
     </row>
-    <row r="35" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="35" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="46"/>
       <c r="C35" s="46"/>
       <c r="D35" s="46"/>
       <c r="F35" s="47"/>
       <c r="N35" s="15"/>
     </row>
-    <row r="36" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="36" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="46"/>
       <c r="C36" s="46"/>
       <c r="D36" s="46"/>
       <c r="F36" s="47"/>
       <c r="N36" s="15"/>
     </row>
-    <row r="37" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="37" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="46"/>
       <c r="C37" s="46"/>
       <c r="D37" s="46"/>
       <c r="F37" s="47"/>
       <c r="N37" s="15"/>
     </row>
-    <row r="38" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="38" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="16"/>
       <c r="B38" s="46"/>
       <c r="C38" s="46"/>
@@ -8606,7 +9182,7 @@
       <c r="F38" s="47"/>
       <c r="N38" s="15"/>
     </row>
-    <row r="39" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="39" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="16"/>
       <c r="B39" s="46"/>
       <c r="C39" s="46"/>
@@ -8614,7 +9190,7 @@
       <c r="F39" s="47"/>
       <c r="N39" s="15"/>
     </row>
-    <row r="40" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="40" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="16"/>
       <c r="B40" s="46"/>
       <c r="C40" s="46"/>
@@ -8622,7 +9198,7 @@
       <c r="F40" s="47"/>
       <c r="N40" s="15"/>
     </row>
-    <row r="41" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="41" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="16"/>
       <c r="B41" s="46"/>
       <c r="C41" s="46"/>
@@ -8655,11 +9231,6 @@
     <oddFooter>&amp;CCopyright © 2005 Lawson  Software Inc. all rights reserved</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId17"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8670,12 +9241,12 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="35.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="48" customWidth="1"/>
@@ -8694,7 +9265,7 @@
     <col min="15" max="16384" width="9.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.5" customHeight="1">
+    <row r="1" spans="1:14" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="80" t="s">
         <v>55</v>
       </c>
@@ -8712,7 +9283,7 @@
       <c r="M1" s="54"/>
       <c r="N1" s="55"/>
     </row>
-    <row r="2" spans="1:14" ht="17.5" customHeight="1">
+    <row r="2" spans="1:14" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="82" t="s">
         <v>56</v>
       </c>
@@ -8730,7 +9301,7 @@
       <c r="M2" s="54"/>
       <c r="N2" s="55"/>
     </row>
-    <row r="3" spans="1:14" s="38" customFormat="1" ht="17" customHeight="1">
+    <row r="3" spans="1:14" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
         <v>14</v>
       </c>
@@ -8743,7 +9314,7 @@
       <c r="F3" s="43"/>
       <c r="N3" s="39"/>
     </row>
-    <row r="4" spans="1:14" s="42" customFormat="1" ht="34.25" customHeight="1">
+    <row r="4" spans="1:14" s="42" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
         <v>43</v>
       </c>
@@ -8787,7 +9358,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="109" customFormat="1" ht="17.5" customHeight="1">
+    <row r="5" spans="1:14" s="109" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="106" t="s">
         <v>36</v>
       </c>
@@ -8831,12 +9402,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="6" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="94">
-        <v>2.13</v>
+      <c r="B6" s="94" t="s">
+        <v>148</v>
       </c>
       <c r="C6" s="95">
         <v>40909</v>
@@ -8875,7 +9446,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1">
+    <row r="7" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="102" t="s">
         <v>80</v>
       </c>
@@ -8919,7 +9490,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="8" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
@@ -8961,12 +9532,12 @@
       </c>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="9" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C9" s="118">
         <v>41576</v>
@@ -9003,7 +9574,7 @@
       </c>
       <c r="N9" s="15"/>
     </row>
-    <row r="10" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="10" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>142</v>
       </c>
@@ -9045,10 +9616,7 @@
       </c>
       <c r="N10" s="15"/>
     </row>
-    <row r="11" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
-      <c r="A11" s="14" t="s">
-        <v>147</v>
-      </c>
+    <row r="11" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
       <c r="D11" s="46"/>
@@ -9056,10 +9624,7 @@
       <c r="H11" s="87"/>
       <c r="N11" s="15"/>
     </row>
-    <row r="12" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
-      <c r="A12" s="14" t="s">
-        <v>148</v>
-      </c>
+    <row r="12" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="46"/>
       <c r="C12" s="46"/>
       <c r="D12" s="46"/>
@@ -9067,10 +9632,7 @@
       <c r="H12" s="87"/>
       <c r="N12" s="15"/>
     </row>
-    <row r="13" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
-      <c r="A13" s="14" t="s">
-        <v>149</v>
-      </c>
+    <row r="13" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
       <c r="D13" s="46"/>
@@ -9078,49 +9640,49 @@
       <c r="H13" s="87"/>
       <c r="N13" s="15"/>
     </row>
-    <row r="14" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="14" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="46"/>
       <c r="C14" s="46"/>
       <c r="D14" s="46"/>
       <c r="F14" s="47"/>
       <c r="N14" s="15"/>
     </row>
-    <row r="15" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="15" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
       <c r="D15" s="46"/>
       <c r="F15" s="47"/>
       <c r="N15" s="15"/>
     </row>
-    <row r="16" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="16" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
       <c r="D16" s="46"/>
       <c r="F16" s="47"/>
       <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="17" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="46"/>
       <c r="C17" s="46"/>
       <c r="D17" s="46"/>
       <c r="F17" s="47"/>
       <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="18" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
       <c r="D18" s="46"/>
       <c r="F18" s="47"/>
       <c r="N18" s="15"/>
     </row>
-    <row r="19" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="19" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
       <c r="D19" s="46"/>
       <c r="F19" s="47"/>
       <c r="N19" s="15"/>
     </row>
-    <row r="20" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="20" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16"/>
       <c r="B20" s="46"/>
       <c r="C20" s="46"/>
@@ -9128,7 +9690,7 @@
       <c r="F20" s="47"/>
       <c r="N20" s="15"/>
     </row>
-    <row r="21" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="21" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="16"/>
       <c r="B21" s="46"/>
       <c r="C21" s="46"/>
@@ -9136,7 +9698,7 @@
       <c r="F21" s="47"/>
       <c r="N21" s="15"/>
     </row>
-    <row r="22" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="22" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="16"/>
       <c r="B22" s="46"/>
       <c r="C22" s="46"/>
@@ -9144,7 +9706,7 @@
       <c r="F22" s="47"/>
       <c r="N22" s="15"/>
     </row>
-    <row r="23" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="23" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="16"/>
       <c r="B23" s="46"/>
       <c r="C23" s="46"/>
@@ -9164,27 +9726,382 @@
     <oddFooter>&amp;CCopyright © 2005 Lawson  Software Inc. all rights reserved</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId4"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="48" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="45.5" style="48" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="12" style="16" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="31.5" style="16" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="16" customWidth="1"/>
+    <col min="14" max="14" width="82.33203125" style="15" customWidth="1"/>
+    <col min="15" max="16384" width="9.1640625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="55"/>
+    </row>
+    <row r="2" spans="1:14" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="82" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="83"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="55"/>
+    </row>
+    <row r="3" spans="1:14" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="78"/>
+      <c r="C3" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="79"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="43"/>
+      <c r="N3" s="39"/>
+    </row>
+    <row r="4" spans="1:14" s="42" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="109" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="106" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="107" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="106" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="108" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="108" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="109" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="107" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="109" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="109" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="108" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="110" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="100" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="95">
+        <v>41882</v>
+      </c>
+      <c r="D6" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="111" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="93" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="93" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="L6" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" s="99" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="13">
+        <v>4</v>
+      </c>
+      <c r="C7" s="95">
+        <v>41882</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="93" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="F8" s="47"/>
+      <c r="H8" s="87"/>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="F9" s="47"/>
+      <c r="H9" s="87"/>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="F10" s="47"/>
+      <c r="H10" s="87"/>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="F16" s="47"/>
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="16"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="F17" s="47"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="16"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="F18" s="47"/>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="16"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="F19" s="47"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="16"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="N20" s="15"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="5" scale="56" fitToWidth="2" orientation="landscape"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;CCopyright © 2005 Lawson  Software Inc. all rights reserved</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>